<commit_message>
GoogleSearch read TestData from Excel
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data.xlsx
+++ b/src/main/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/onceclick/CODE/PERSONAL/training/automation-test/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF62182-528C-0749-8E60-ECFF9B836512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9CF3C5-589C-FE42-B055-78BBB8E66144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{ADC41698-933C-FF41-8072-8B21F4B780BA}"/>
   </bookViews>
@@ -67,9 +67,6 @@
     <t>PALTGC0TST</t>
   </si>
   <si>
-    <t>keyword</t>
-  </si>
-  <si>
     <t>POI Reading and Writing Excel file in Java</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>TestNG Annotations</t>
+  </si>
+  <si>
+    <t>keywords</t>
   </si>
 </sst>
 </file>
@@ -587,7 +587,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,7 +601,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -609,7 +609,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -617,7 +617,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -625,7 +625,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -633,7 +633,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>